<commit_message>
#47 - Rubah format impor
</commit_message>
<xml_diff>
--- a/storage/app/public/template_upload/Format_Upload_AKI_&_AKB.xlsx
+++ b/storage/app/public/template_upload/Format_Upload_AKI_&_AKB.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\OpenDK\storage\app\public\template_upload\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBD26F4E-082C-4465-A17E-18A83E8ED2FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FORM AKI &amp; AKB" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>jumlah_aki</t>
   </si>
@@ -25,13 +31,37 @@
   </si>
   <si>
     <t>desa_id</t>
+  </si>
+  <si>
+    <t>53.06.13.2021</t>
+  </si>
+  <si>
+    <t>53.06.13.2020</t>
+  </si>
+  <si>
+    <t>53.06.13.2019</t>
+  </si>
+  <si>
+    <t>53.06.13.2018</t>
+  </si>
+  <si>
+    <t>53.06.13.2017</t>
+  </si>
+  <si>
+    <t>53.06.13.2016</t>
+  </si>
+  <si>
+    <t>53.06.13.2015</t>
+  </si>
+  <si>
+    <t>53.06.13.2014</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -84,6 +114,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -130,7 +168,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -162,9 +200,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -196,6 +252,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -371,21 +445,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -396,9 +470,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1">
-        <v>5203090011</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="B2" s="1">
         <v>23</v>
@@ -407,9 +481,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1">
-        <v>5203090012</v>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
@@ -418,9 +492,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1">
-        <v>5203090013</v>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="B4" s="1">
         <v>343</v>
@@ -429,9 +503,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1">
-        <v>5203090014</v>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="B5" s="1">
         <v>6</v>
@@ -440,9 +514,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1">
-        <v>5203090015</v>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B6" s="1">
         <v>23</v>
@@ -451,9 +525,9 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="1">
-        <v>5203090016</v>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="B7" s="1">
         <v>3</v>
@@ -462,9 +536,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="1">
-        <v>5203090017</v>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B8" s="1">
         <v>23</v>
@@ -473,9 +547,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
-      <c r="A9" s="1">
-        <v>5203090018</v>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B9" s="1">
         <v>4</v>
@@ -490,24 +564,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>